<commit_message>
& - 80533184 от 05.08.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Cyprus/#EURO#Cyprus#Commemorative#[2009-present]#UNC%varieties.xlsx
+++ b/Collections/EURO/Cyprus/#EURO#Cyprus#Commemorative#[2009-present]#UNC%varieties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Cyprus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9990C4A7-5EEE-49A6-BF1E-E1924279F107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17876CF8-2A6F-4A32-9C0C-9543235AD327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="33150" windowHeight="17700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="44">
   <si>
     <t>Year</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>Subtype_2#Special_marks_1</t>
+  </si>
+  <si>
+    <t>20th Anniversary - Cyprus' accession to the European Union</t>
+  </si>
+  <si>
+    <t>7.000</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -302,6 +308,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -450,7 +464,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -539,13 +553,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -760,9 +793,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1037,7 +1070,7 @@
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1594,32 +1627,30 @@
       <c r="A18" s="6">
         <v>2024</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>4</v>
+      <c r="B18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H18" s="9" t="s">
-        <v>4</v>
+      <c r="H18" s="9">
+        <v>0</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>4</v>
       </c>
       <c r="J18" s="10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J18" si="5">IF(OR(AND(H18&gt;1,H18&lt;&gt;"-"),AND(I18&gt;1,I18&lt;&gt;"-")),"Can exchange","")</f>
         <v/>
       </c>
     </row>
@@ -1640,11 +1671,45 @@
     <mergeCell ref="C1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="H6:I6 H3:H5 H11:I11">
+    <cfRule type="containsText" dxfId="27" priority="61" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6:I6 H3:H5 H11:I11">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="containsText" dxfId="26" priority="59" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I5">
     <cfRule type="containsText" dxfId="25" priority="57" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6:I6 H3:H5 H11:I11">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I5">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1656,12 +1721,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+  <conditionalFormatting sqref="H7">
     <cfRule type="containsText" dxfId="24" priority="55" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1673,12 +1738,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I5">
+  <conditionalFormatting sqref="I7">
     <cfRule type="containsText" dxfId="23" priority="53" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I4))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I5">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I7))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1690,12 +1755,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+  <conditionalFormatting sqref="H8">
     <cfRule type="containsText" dxfId="22" priority="51" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H7))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1707,12 +1772,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+  <conditionalFormatting sqref="I8">
     <cfRule type="containsText" dxfId="21" priority="49" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I7))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1724,46 +1789,46 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="containsText" dxfId="20" priority="47" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="containsText" dxfId="19" priority="45" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I8))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H9:I9">
+    <cfRule type="containsText" dxfId="20" priority="43" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9:I9">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="19" priority="41" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
     <cfRule type="containsText" dxfId="18" priority="39" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H9:I9">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1775,12 +1840,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="H12">
     <cfRule type="containsText" dxfId="17" priority="37" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1792,12 +1857,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
+  <conditionalFormatting sqref="I12">
     <cfRule type="containsText" dxfId="16" priority="35" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1809,12 +1874,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+  <conditionalFormatting sqref="H13">
     <cfRule type="containsText" dxfId="15" priority="33" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1826,12 +1891,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="I13">
     <cfRule type="containsText" dxfId="14" priority="31" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I12))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1843,46 +1908,46 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="containsText" dxfId="13" priority="29" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="12" priority="27" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I13))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H14:I14">
+    <cfRule type="containsText" dxfId="13" priority="25" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:I14">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
     <cfRule type="containsText" dxfId="11" priority="21" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H14))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:I14">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1894,12 +1959,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+  <conditionalFormatting sqref="I16">
     <cfRule type="containsText" dxfId="10" priority="19" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1911,29 +1976,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I15))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="8" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
+  <conditionalFormatting sqref="I17">
+    <cfRule type="containsText" dxfId="9" priority="15" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I17">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1945,12 +1993,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I17))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I17">
+  <conditionalFormatting sqref="H16">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1962,30 +2010,30 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H16))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I18">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1997,28 +2045,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H18))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(I18))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -2041,7 +2072,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>